<commit_message>
validate_url function added. added new login validation.
</commit_message>
<xml_diff>
--- a/resources/admission.xlsx
+++ b/resources/admission.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="166">
   <si>
     <t>Xpath</t>
   </si>
@@ -505,6 +505,15 @@
   </si>
   <si>
     <t>Submit</t>
+  </si>
+  <si>
+    <t>Redirect</t>
+  </si>
+  <si>
+    <t>validate_url</t>
+  </si>
+  <si>
+    <t>http://104.196.248.241:9999/#/welcome</t>
   </si>
 </sst>
 </file>
@@ -856,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15"/>
@@ -980,53 +989,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30">
       <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -1042,19 +1042,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -1062,16 +1062,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1085,16 +1082,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1108,16 +1105,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1131,13 +1128,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1151,36 +1151,33 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -1194,13 +1191,16 @@
     </row>
     <row r="16" spans="1:7" ht="30">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1214,119 +1214,116 @@
     </row>
     <row r="17" spans="1:7" ht="30">
       <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30">
+      <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30">
+      <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60">
+      <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="75">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75">
+      <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45">
+      <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="2">
-        <v>123456</v>
+      <c r="D22" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -1340,13 +1337,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D23" s="2">
+        <v>123456</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -1360,10 +1360,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>9</v>
@@ -1380,16 +1380,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>153</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -1403,62 +1400,65 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30">
-      <c r="A27" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30">
+      <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E28" s="1">
         <v>1</v>
       </c>
       <c r="F28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -1466,50 +1466,50 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30">
-      <c r="A30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30">
+      <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>9</v>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>9</v>
@@ -1549,7 +1549,7 @@
         <v>69</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>9</v>
@@ -1566,56 +1566,53 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-      <c r="G34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30">
-      <c r="A35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30">
+      <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="75">
-      <c r="A36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -1629,16 +1626,16 @@
     </row>
     <row r="37" spans="1:7" ht="75">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="2">
-        <v>123456</v>
+      <c r="D37" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -1652,16 +1649,16 @@
     </row>
     <row r="38" spans="1:7" ht="75">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>57</v>
+      <c r="D38" s="2">
+        <v>123456</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -1675,16 +1672,16 @@
     </row>
     <row r="39" spans="1:7" ht="75">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>94</v>
+      <c r="D39" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -1698,16 +1695,16 @@
     </row>
     <row r="40" spans="1:7" ht="75">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -1721,16 +1718,16 @@
     </row>
     <row r="41" spans="1:7" ht="75">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -1744,79 +1741,79 @@
     </row>
     <row r="42" spans="1:7" ht="75">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="75">
+      <c r="A43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E42" s="1">
-        <v>1</v>
-      </c>
-      <c r="F42" s="1">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="30">
-      <c r="A43" s="1" t="s">
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="60">
+      <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="75">
-      <c r="A44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="75">
+      <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="1">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -1830,13 +1827,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -1850,10 +1850,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>9</v>
@@ -1870,145 +1870,142 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="1">
-        <v>1</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30">
-      <c r="A49" s="1" t="s">
+      <c r="C49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30">
+      <c r="A50" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="1">
-        <v>1</v>
-      </c>
-      <c r="F49" s="1">
-        <v>1</v>
-      </c>
-      <c r="G49" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="75">
-      <c r="A50" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="75">
+      <c r="A51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" s="1">
-        <v>1</v>
-      </c>
-      <c r="F50" s="1">
-        <v>1</v>
-      </c>
-      <c r="G50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="90">
-      <c r="A51" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="90">
+      <c r="A52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E51" s="1">
-        <v>1</v>
-      </c>
-      <c r="F51" s="1">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="75">
-      <c r="A52" s="1" t="s">
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="75">
+      <c r="A53" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="1">
-        <v>1</v>
-      </c>
-      <c r="F52" s="1">
-        <v>1</v>
-      </c>
-      <c r="G52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45">
-      <c r="A53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45">
+      <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" s="1">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1">
-        <v>1</v>
-      </c>
-      <c r="G53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
@@ -2022,36 +2019,36 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="1">
-        <v>1</v>
-      </c>
-      <c r="F55" s="1">
-        <v>1</v>
-      </c>
-      <c r="G55" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -2065,16 +2062,16 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -2088,99 +2085,99 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="1">
-        <v>1</v>
-      </c>
-      <c r="F58" s="1">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="30">
-      <c r="A59" s="1" t="s">
+      <c r="C59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30">
+      <c r="A60" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="1">
-        <v>1</v>
-      </c>
-      <c r="F59" s="1">
-        <v>1</v>
-      </c>
-      <c r="G59" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="4" t="s">
+      <c r="C60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="1">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1">
-        <v>1</v>
-      </c>
-      <c r="G60" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="30">
-      <c r="A61" s="1" t="s">
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30">
+      <c r="A62" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="1">
-        <v>1</v>
-      </c>
-      <c r="F61" s="1">
-        <v>1</v>
-      </c>
-      <c r="G61" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="90">
-      <c r="A62" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>133</v>
+        <v>9</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
@@ -2194,16 +2191,16 @@
     </row>
     <row r="63" spans="1:7" ht="90">
       <c r="A63" s="1" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>134</v>
+      <c r="D63" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -2217,16 +2214,16 @@
     </row>
     <row r="64" spans="1:7" ht="90">
       <c r="A64" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>117</v>
+      <c r="D64" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="E64" s="1">
         <v>1</v>
@@ -2240,16 +2237,16 @@
     </row>
     <row r="65" spans="1:7" ht="90">
       <c r="A65" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>87</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -2263,16 +2260,16 @@
     </row>
     <row r="66" spans="1:7" ht="90">
       <c r="A66" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>101</v>
+      <c r="D66" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -2286,59 +2283,59 @@
     </row>
     <row r="67" spans="1:7" ht="90">
       <c r="A67" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D67" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="90">
+      <c r="A68" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D68" s="4">
         <v>123123</v>
       </c>
-      <c r="E67" s="1">
-        <v>1</v>
-      </c>
-      <c r="F67" s="1">
-        <v>1</v>
-      </c>
-      <c r="G67" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="75">
-      <c r="A68" s="1" t="s">
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="75">
+      <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="1">
-        <v>1</v>
-      </c>
-      <c r="F68" s="1">
-        <v>1</v>
-      </c>
-      <c r="G68" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="C69" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="E69" s="1">
         <v>1</v>
@@ -2352,10 +2349,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>17</v>
@@ -2375,10 +2372,10 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>17</v>
@@ -2396,46 +2393,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="30">
+    <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="30">
+      <c r="A73" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="1">
-        <v>1</v>
-      </c>
-      <c r="F72" s="1">
-        <v>1</v>
-      </c>
-      <c r="G72" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="90">
-      <c r="A73" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="C73" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>144</v>
+        <v>9</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="90">
       <c r="A74" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>87</v>
@@ -2446,10 +2452,10 @@
     </row>
     <row r="75" spans="1:7" ht="90">
       <c r="A75" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>87</v>
@@ -2458,23 +2464,37 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30">
+    <row r="76" spans="1:7" ht="90">
       <c r="A76" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="30">
+      <c r="A77" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="1">
-        <v>1</v>
-      </c>
-      <c r="F76" s="1">
-        <v>1</v>
-      </c>
-      <c r="G76" s="1">
+      <c r="C77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update reporting and running the project will now do all the test . Currently there are 2 test available Login and Admission. Admission right now has a lot of issue on the xpath since there has been changes on the element on the site and it needs to update.
</commit_message>
<xml_diff>
--- a/resources/admission.xlsx
+++ b/resources/admission.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="180">
   <si>
     <t>Xpath</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>/html/body/div/div/md-content/div/section/div[7]/button</t>
-  </si>
-  <si>
     <t>Operation</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>qa.test1@cvhcare.com</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -300,12 +294,6 @@
     <t>Mar 10, 2017</t>
   </si>
   <si>
-    <t>Jenny, Duque</t>
-  </si>
-  <si>
-    <t>Jennifer, Cortez</t>
-  </si>
-  <si>
     <t>Patient is at Home</t>
   </si>
   <si>
@@ -315,9 +303,6 @@
     <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[1]/md-card[1]/md-card-content[1]/span[1]</t>
   </si>
   <si>
-    <t>Hamoudi, Al Bander</t>
-  </si>
-  <si>
     <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-expanded/md-expansion-panel-content/div[1]/md-card[1]/md-card-content[1]/span[3]/span[1]</t>
   </si>
   <si>
@@ -375,9 +360,6 @@
     <t>5465225</t>
   </si>
   <si>
-    <t>313</t>
-  </si>
-  <si>
     <t>HIC Number</t>
   </si>
   <si>
@@ -462,65 +444,125 @@
     <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-content/md-expansion-panel-group/md-expansion-panel[2]/md-expansion-panel-collapsed/md-icon</t>
   </si>
   <si>
+    <t>//*[@id="select_53"]</t>
+  </si>
+  <si>
+    <t>Select first</t>
+  </si>
+  <si>
+    <t>Select First</t>
+  </si>
+  <si>
+    <t>Cortez</t>
+  </si>
+  <si>
+    <t>//*[@id="select_60"]</t>
+  </si>
+  <si>
+    <t>/html/body/md-backdrop</t>
+  </si>
+  <si>
+    <t>clcose background</t>
+  </si>
+  <si>
+    <t>//*[@id="select_68"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_84"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_85"]</t>
+  </si>
+  <si>
+    <t>//*[@id="input_86"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-actions/button[2]</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Redirect</t>
+  </si>
+  <si>
+    <t>validate_url</t>
+  </si>
+  <si>
+    <t>Clarissa, Cortez</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
     <t>//*[@id="ul-48"]/li[1]</t>
   </si>
   <si>
-    <t>//*[@id="select_53"]</t>
-  </si>
-  <si>
-    <t>Select first</t>
-  </si>
-  <si>
-    <t>Select First</t>
-  </si>
-  <si>
-    <t>Duque</t>
-  </si>
-  <si>
-    <t>Cortez</t>
-  </si>
-  <si>
-    <t>//*[@id="select_60"]</t>
-  </si>
-  <si>
-    <t>/html/body/md-backdrop</t>
-  </si>
-  <si>
-    <t>clcose background</t>
-  </si>
-  <si>
-    <t>//*[@id="select_68"]</t>
-  </si>
-  <si>
-    <t>//*[@id="input_84"]</t>
-  </si>
-  <si>
-    <t>//*[@id="input_85"]</t>
-  </si>
-  <si>
-    <t>//*[@id="input_86"]</t>
-  </si>
-  <si>
-    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-actions/button[2]</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
-    <t>Redirect</t>
-  </si>
-  <si>
-    <t>validate_url</t>
-  </si>
-  <si>
-    <t>http://104.196.248.241:9999/#/welcome</t>
+    <t>Andres, Anacker</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/md-content/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item[3]</t>
+  </si>
+  <si>
+    <t>In Approval Tab</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/md-content/div[3]/md-content/div/div/div/div[1]/button[1]</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/md-content/div[3]/md-content/div/div/div/div[2]/form/input</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>Start SOC</t>
+  </si>
+  <si>
+    <t>User Menu</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-toolbar/div/md-menu/button</t>
+  </si>
+  <si>
+    <t>//*[@id="menu_container_3"]/md-menu-content/md-menu-item[2]/a</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/div/md-card/md-card-actions/button[1]</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/md-content/div[3]/md-content/md-list/md-list-item/div/button</t>
+  </si>
+  <si>
+    <t>Select 1st Patient</t>
+  </si>
+  <si>
+    <t>Search Bar</t>
+  </si>
+  <si>
+    <t>http://104.198.15.201:9999/#/welcome</t>
+  </si>
+  <si>
+    <t>http://104.198.15.201:9999/#/login</t>
+  </si>
+  <si>
+    <t>intake.user1@cvhcare.com</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/div/section/div[8]/button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +574,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -552,10 +601,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -571,8 +624,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -865,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15"/>
@@ -897,24 +954,24 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -928,16 +985,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -951,13 +1008,13 @@
     </row>
     <row r="4" spans="1:7" ht="48.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -971,13 +1028,13 @@
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -991,24 +1048,24 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30">
+        <v>156</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -1022,13 +1079,13 @@
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1042,13 +1099,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1062,13 +1119,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1082,16 +1139,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1105,16 +1162,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1128,16 +1185,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1151,13 +1208,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1171,13 +1228,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -1191,16 +1248,16 @@
     </row>
     <row r="16" spans="1:7" ht="30">
       <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1214,13 +1271,13 @@
     </row>
     <row r="17" spans="1:7" ht="30">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -1234,13 +1291,13 @@
     </row>
     <row r="18" spans="1:7" ht="30">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -1254,13 +1311,13 @@
     </row>
     <row r="19" spans="1:7" ht="30">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -1274,13 +1331,13 @@
     </row>
     <row r="20" spans="1:7" ht="60">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -1294,13 +1351,13 @@
     </row>
     <row r="21" spans="1:7" ht="75">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -1314,16 +1371,16 @@
     </row>
     <row r="22" spans="1:7" ht="45">
       <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -1337,16 +1394,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="2">
-        <v>123456</v>
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -1360,13 +1417,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -1380,13 +1437,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -1400,16 +1457,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1423,13 +1480,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -1443,16 +1500,16 @@
     </row>
     <row r="28" spans="1:7" ht="30">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1466,19 +1523,19 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
       <c r="F29" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -1486,13 +1543,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -1506,13 +1563,13 @@
     </row>
     <row r="31" spans="1:7" ht="30">
       <c r="A31" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -1526,13 +1583,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -1546,13 +1603,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -1566,13 +1623,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -1586,13 +1643,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -1606,13 +1663,13 @@
     </row>
     <row r="36" spans="1:7" ht="30">
       <c r="A36" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -1626,16 +1683,16 @@
     </row>
     <row r="37" spans="1:7" ht="75">
       <c r="A37" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -1649,13 +1706,13 @@
     </row>
     <row r="38" spans="1:7" ht="75">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D38" s="2">
         <v>123456</v>
@@ -1672,16 +1729,16 @@
     </row>
     <row r="39" spans="1:7" ht="75">
       <c r="A39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -1695,16 +1752,16 @@
     </row>
     <row r="40" spans="1:7" ht="75">
       <c r="A40" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -1718,16 +1775,16 @@
     </row>
     <row r="41" spans="1:7" ht="75">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -1741,16 +1798,16 @@
     </row>
     <row r="42" spans="1:7" ht="75">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -1764,16 +1821,16 @@
     </row>
     <row r="43" spans="1:7" ht="75">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -1787,13 +1844,13 @@
     </row>
     <row r="44" spans="1:7" ht="60">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -1807,13 +1864,13 @@
     </row>
     <row r="45" spans="1:7" ht="75">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -1827,16 +1884,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -1850,13 +1907,13 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -1870,13 +1927,13 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -1890,13 +1947,13 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -1910,13 +1967,13 @@
     </row>
     <row r="50" spans="1:7" ht="30">
       <c r="A50" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
@@ -1930,16 +1987,16 @@
     </row>
     <row r="51" spans="1:7" ht="75">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="E51" s="1">
         <v>1</v>
@@ -1953,16 +2010,16 @@
     </row>
     <row r="52" spans="1:7" ht="90">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -1976,13 +2033,13 @@
     </row>
     <row r="53" spans="1:7" ht="75">
       <c r="A53" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53" s="1">
         <v>1</v>
@@ -1996,16 +2053,16 @@
     </row>
     <row r="54" spans="1:7" ht="45">
       <c r="A54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D54" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
@@ -2019,16 +2076,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -2042,13 +2099,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -2062,16 +2119,16 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -2085,16 +2142,16 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="E58" s="1">
         <v>1</v>
@@ -2108,13 +2165,13 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
@@ -2128,13 +2185,13 @@
     </row>
     <row r="60" spans="1:7" ht="30">
       <c r="A60" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1">
         <v>1</v>
@@ -2148,16 +2205,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
@@ -2171,13 +2228,13 @@
     </row>
     <row r="62" spans="1:7" ht="30">
       <c r="A62" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
@@ -2191,16 +2248,16 @@
     </row>
     <row r="63" spans="1:7" ht="90">
       <c r="A63" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -2214,16 +2271,16 @@
     </row>
     <row r="64" spans="1:7" ht="90">
       <c r="A64" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E64" s="1">
         <v>1</v>
@@ -2237,16 +2294,16 @@
     </row>
     <row r="65" spans="1:7" ht="90">
       <c r="A65" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -2260,16 +2317,16 @@
     </row>
     <row r="66" spans="1:7" ht="90">
       <c r="A66" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -2283,16 +2340,16 @@
     </row>
     <row r="67" spans="1:7" ht="90">
       <c r="A67" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E67" s="1">
         <v>1</v>
@@ -2306,13 +2363,13 @@
     </row>
     <row r="68" spans="1:7" ht="90">
       <c r="A68" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D68" s="4">
         <v>123123</v>
@@ -2329,13 +2386,13 @@
     </row>
     <row r="69" spans="1:7" ht="75">
       <c r="A69" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E69" s="1">
         <v>1</v>
@@ -2349,16 +2406,16 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E70" s="1">
         <v>1</v>
@@ -2372,16 +2429,16 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E71" s="1">
         <v>1</v>
@@ -2395,16 +2452,16 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E72" s="1">
         <v>1</v>
@@ -2418,13 +2475,13 @@
     </row>
     <row r="73" spans="1:7" ht="30">
       <c r="A73" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E73" s="1">
         <v>1</v>
@@ -2438,69 +2495,234 @@
     </row>
     <row r="74" spans="1:7" ht="90">
       <c r="A74" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="90">
       <c r="A75" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="90">
       <c r="A76" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30">
       <c r="A77" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="45">
+      <c r="A78" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="1">
-        <v>1</v>
-      </c>
-      <c r="F77" s="1">
-        <v>1</v>
-      </c>
-      <c r="G77" s="1">
+      <c r="C78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30">
+      <c r="A79" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="30">
+      <c r="A80" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30">
+      <c r="A81" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1">
+        <v>3</v>
+      </c>
+      <c r="G81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="30">
+      <c r="A82" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1">
+        <v>1</v>
+      </c>
+      <c r="G82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="30">
+      <c r="B84" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+      <c r="F84" s="1">
+        <v>1</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30">
+      <c r="A85" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+      <c r="F85" s="1">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D85" r:id="rId1" location="/login"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>